<commit_message>
backup de atualização de códigos
</commit_message>
<xml_diff>
--- a/data/icva.xlsx
+++ b/data/icva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Aviso,Comunicado ao Mercado e Fato\Comunicado ao Mercado - ICVA\2020\10 Outubro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Aviso,Comunicado ao Mercado e Fato\Comunicado ao Mercado - ICVA\2021\1 Janeiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -425,22 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E95"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -457,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>41275</v>
       </c>
@@ -474,7 +474,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>41306</v>
       </c>
@@ -491,7 +491,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>41334</v>
       </c>
@@ -508,7 +508,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>41365</v>
       </c>
@@ -525,7 +525,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>41395</v>
       </c>
@@ -542,7 +542,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>41426</v>
       </c>
@@ -559,7 +559,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>41456</v>
       </c>
@@ -576,7 +576,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>41487</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>41518</v>
       </c>
@@ -610,7 +610,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>41548</v>
       </c>
@@ -627,7 +627,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>41579</v>
       </c>
@@ -644,7 +644,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>41609</v>
       </c>
@@ -661,7 +661,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>41640</v>
       </c>
@@ -678,7 +678,7 @@
         <v>8.3556304359949207E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>41671</v>
       </c>
@@ -695,7 +695,7 @@
         <v>8.5838857838311355E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>41699</v>
       </c>
@@ -712,7 +712,7 @@
         <v>5.0449535072922158E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>41730</v>
       </c>
@@ -729,7 +729,7 @@
         <v>6.4330273867492016E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>41760</v>
       </c>
@@ -746,7 +746,7 @@
         <v>5.0724347806078152E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>41791</v>
       </c>
@@ -763,7 +763,7 @@
         <v>3.097969982497073E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>41821</v>
       </c>
@@ -780,7 +780,7 @@
         <v>3.6779756914917749E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>41852</v>
       </c>
@@ -797,7 +797,7 @@
         <v>4.2794843400101534E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>41883</v>
       </c>
@@ -814,7 +814,7 @@
         <v>2.85077558272262E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>41913</v>
       </c>
@@ -831,7 +831,7 @@
         <v>2.132053095079911E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>41944</v>
       </c>
@@ -848,7 +848,7 @@
         <v>2.5467920155174184E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>41974</v>
       </c>
@@ -865,7 +865,7 @@
         <v>1.8395128697253904E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>42005</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1.4754402087671314E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>42036</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2.4661885329642086E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>42064</v>
       </c>
@@ -916,7 +916,7 @@
         <v>1.5851957239666481E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>42095</v>
       </c>
@@ -933,7 +933,7 @@
         <v>-4.8686486477544921E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>42125</v>
       </c>
@@ -950,7 +950,7 @@
         <v>6.9802854307985385E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>42156</v>
       </c>
@@ -967,7 +967,7 @@
         <v>5.9453867762737644E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>42186</v>
       </c>
@@ -984,7 +984,7 @@
         <v>-1.1420841226051026E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>42217</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>-2.29475701955838E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>42248</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>-3.0443940388387047E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>42278</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>-3.7676544485519048E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>42309</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>-4.3798138403188136E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>42339</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>-5.9292451959600201E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>42370</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>-5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>42401</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>-6.2135709595451671E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>42430</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>-5.8323766673473498E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>42461</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>-6.0895609387856542E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42491</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>-4.4730708878269576E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>42522</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>-3.2926023001528137E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>42552</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>-3.9160765044360946E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>42583</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>-5.094406235449167E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>42614</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>-5.0870996353320819E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>42644</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>-5.1257021572631012E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>42675</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>-4.933249588677957E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>42705</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>-5.6111038938339797E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>42736</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>-4.3293409485345768E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>42767</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>-1.0551641727187921E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>42795</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>-2.209327422366214E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>42826</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>2.6264196506697868E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>42856</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>-1.6064414031452312E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>42887</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>-6.4156773386371269E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>42917</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7.528273846723943E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>42948</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>1.0725572276793383E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>42979</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>6.7506931383911617E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>43009</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>7.1515874765988308E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>43040</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>2.5743820948904705E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>43070</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>1.6720486463239537E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>43101</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>1.8731381080357545E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>43132</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>1.4877158546585667E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>43160</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>2.1525690736809544E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>43191</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>2.6306931915095255E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>43221</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>43252</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>43282</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>43313</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>43344</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>43374</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>43405</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>43435</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>43466</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>43517</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>43525</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>43556</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>43586</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>43617</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>43647</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>43678</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>43709</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>43739</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>43770</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>43800</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>43831</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>43862</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>3.7000000000000005E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>43891</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>43922</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>-0.371</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>43952</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>43983</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>-0.249</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>44013</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>-0.20699999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>44044</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>44075</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>-7.400000000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>44105</v>
       </c>
@@ -2053,6 +2053,57 @@
       </c>
       <c r="E95" s="4">
         <v>-8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="3">
+        <v>44136</v>
+      </c>
+      <c r="B96" s="4">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="C96" s="4">
+        <v>-2.1000000000000001E-2</v>
+      </c>
+      <c r="D96" s="4">
+        <v>-0.11</v>
+      </c>
+      <c r="E96" s="4">
+        <v>-0.09</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="3">
+        <v>44166</v>
+      </c>
+      <c r="B97" s="4">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="C97" s="4">
+        <v>-4.5999999999999999E-2</v>
+      </c>
+      <c r="D97" s="4">
+        <v>-9.8000000000000004E-2</v>
+      </c>
+      <c r="E97" s="4">
+        <v>-0.109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
+        <v>44197</v>
+      </c>
+      <c r="B98" s="4">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="C98" s="4">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="D98" s="4">
+        <v>-0.126</v>
+      </c>
+      <c r="E98" s="4">
+        <v>-0.10299999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small improvements in econ_activity ETL
</commit_message>
<xml_diff>
--- a/data/icva.xlsx
+++ b/data/icva.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Aviso,Comunicado ao Mercado e Fato\Comunicado ao Mercado - ICVA\2021\1 Janeiro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Aviso,Comunicado ao Mercado e Fato\Comunicado ao Mercado - ICVA\2021\2 Fevereiro\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -425,22 +425,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="I95" sqref="I95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -457,7 +457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>41275</v>
       </c>
@@ -474,7 +474,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>41306</v>
       </c>
@@ -491,7 +491,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>41334</v>
       </c>
@@ -508,7 +508,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>41365</v>
       </c>
@@ -525,7 +525,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>41395</v>
       </c>
@@ -542,7 +542,7 @@
         <v>6.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>41426</v>
       </c>
@@ -559,7 +559,7 @@
         <v>6.6000000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>41456</v>
       </c>
@@ -576,7 +576,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>41487</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41518</v>
       </c>
@@ -610,7 +610,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>41548</v>
       </c>
@@ -627,7 +627,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>41579</v>
       </c>
@@ -644,7 +644,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>41609</v>
       </c>
@@ -661,7 +661,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>41640</v>
       </c>
@@ -678,7 +678,7 @@
         <v>8.3556304359949207E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>41671</v>
       </c>
@@ -695,7 +695,7 @@
         <v>8.5838857838311355E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>41699</v>
       </c>
@@ -712,7 +712,7 @@
         <v>5.0449535072922158E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>41730</v>
       </c>
@@ -729,7 +729,7 @@
         <v>6.4330273867492016E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>41760</v>
       </c>
@@ -746,7 +746,7 @@
         <v>5.0724347806078152E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41791</v>
       </c>
@@ -763,7 +763,7 @@
         <v>3.097969982497073E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>41821</v>
       </c>
@@ -780,7 +780,7 @@
         <v>3.6779756914917749E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>41852</v>
       </c>
@@ -797,7 +797,7 @@
         <v>4.2794843400101534E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41883</v>
       </c>
@@ -814,7 +814,7 @@
         <v>2.85077558272262E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41913</v>
       </c>
@@ -831,7 +831,7 @@
         <v>2.132053095079911E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>41944</v>
       </c>
@@ -848,7 +848,7 @@
         <v>2.5467920155174184E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>41974</v>
       </c>
@@ -865,7 +865,7 @@
         <v>1.8395128697253904E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>42005</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1.4754402087671314E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>42036</v>
       </c>
@@ -899,7 +899,7 @@
         <v>2.4661885329642086E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>42064</v>
       </c>
@@ -916,7 +916,7 @@
         <v>1.5851957239666481E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>42095</v>
       </c>
@@ -933,7 +933,7 @@
         <v>-4.8686486477544921E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>42125</v>
       </c>
@@ -950,7 +950,7 @@
         <v>6.9802854307985385E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>42156</v>
       </c>
@@ -967,7 +967,7 @@
         <v>5.9453867762737644E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>42186</v>
       </c>
@@ -984,7 +984,7 @@
         <v>-1.1420841226051026E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>42217</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>-2.29475701955838E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>42248</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>-3.0443940388387047E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>42278</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>-3.7676544485519048E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>42309</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>-4.3798138403188136E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>42339</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>-5.9292451959600201E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>42370</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>-5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>42401</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>-6.2135709595451671E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>42430</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>-5.8323766673473498E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>42461</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>-6.0895609387856542E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>42491</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>-4.4730708878269576E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42522</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>-3.2926023001528137E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>42552</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>-3.9160765044360946E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>42583</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>-5.094406235449167E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>42614</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>-5.0870996353320819E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>42644</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>-5.1257021572631012E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>42675</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>-4.933249588677957E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>42705</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>-5.6111038938339797E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>42736</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>-4.3293409485345768E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>42767</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>-1.0551641727187921E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>42795</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>-2.209327422366214E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>42826</v>
       </c>
@@ -1341,7 +1341,7 @@
         <v>2.6264196506697868E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>42856</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>-1.6064414031452312E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>42887</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>-6.4156773386371269E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>42917</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>7.528273846723943E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>42948</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>1.0725572276793383E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>42979</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>6.7506931383911617E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>43009</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>7.1515874765988308E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>43040</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>2.5743820948904705E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>43070</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>1.6720486463239537E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>43101</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>1.8731381080357545E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>43132</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>1.4877158546585667E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>43160</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>2.1525690736809544E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>43191</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>2.6306931915095255E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>43221</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>43252</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>43282</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>43313</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>43344</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>43374</v>
       </c>
@@ -1647,7 +1647,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>43405</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>43435</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>43466</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>43517</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>43525</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>43556</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>43586</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>43617</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>43647</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>43678</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>43709</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>43739</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>3.9E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>43770</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>43800</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>43831</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>43862</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>3.7000000000000005E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>43891</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>43922</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>-0.371</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>43952</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>-0.29399999999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>43983</v>
       </c>
@@ -1987,7 +1987,7 @@
         <v>-0.249</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>44013</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>-0.20699999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>44044</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>-0.125</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>44075</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>-7.400000000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>44105</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>-8.4000000000000005E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>44136</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>-0.09</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>44166</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>-0.109</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>44197</v>
       </c>
@@ -2104,6 +2104,23 @@
       </c>
       <c r="E98" s="4">
         <v>-0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>44228</v>
+      </c>
+      <c r="B99" s="4">
+        <v>-9.9000000000000005E-2</v>
+      </c>
+      <c r="C99" s="4">
+        <v>-7.1999999999999995E-2</v>
+      </c>
+      <c r="D99" s="4">
+        <v>-0.17100000000000001</v>
+      </c>
+      <c r="E99" s="4">
+        <v>-0.121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>